<commit_message>
Adding new images as inputs for Overlapping model for analysis
</commit_message>
<xml_diff>
--- a/Analysis/TilingVsMarkovTiming.xlsx
+++ b/Analysis/TilingVsMarkovTiming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School_Git\WFCProject\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A1B6D9-2E7A-4B51-9934-B5D2E1F8ADFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52763344-B01A-4225-958B-2B2B34939B22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -489,7 +489,7 @@
   <dimension ref="B2:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>